<commit_message>
unit tests for EPOCH, DY, and BLFL methods, changes to read_edc_tbls(), updated README, example data, documentation
</commit_message>
<xml_diff>
--- a/inst/extdata/spec.xlsx
+++ b/inst/extdata/spec.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t xml:space="preserve">Dataset</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t xml:space="preserve">Data Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Length</t>
   </si>
   <si>
     <t xml:space="preserve">STUDYID</t>
@@ -547,6 +550,9 @@
       <c r="E1" t="s">
         <v>11</v>
       </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -556,13 +562,16 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="F2" t="n">
+        <v>200</v>
       </c>
     </row>
     <row r="3">
@@ -573,13 +582,16 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
+      <c r="F3" t="n">
+        <v>200</v>
       </c>
     </row>
     <row r="4">
@@ -590,13 +602,16 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="F4" t="n">
+        <v>200</v>
       </c>
     </row>
     <row r="5">
@@ -607,13 +622,16 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="F5" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="6">
@@ -624,13 +642,16 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="F6" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="7">
@@ -641,13 +662,16 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="F7" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="8">
@@ -658,13 +682,16 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E8" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="F8" t="n">
+        <v>200</v>
       </c>
     </row>
     <row r="9">
@@ -675,13 +702,16 @@
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E9" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -692,13 +722,16 @@
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E10" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="F10" t="n">
+        <v>200</v>
       </c>
     </row>
     <row r="11">
@@ -709,13 +742,16 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E11" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="F11" t="n">
+        <v>200</v>
       </c>
     </row>
     <row r="12">
@@ -726,13 +762,16 @@
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E12" t="s">
-        <v>36</v>
+        <v>37</v>
+      </c>
+      <c r="F12" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="13">
@@ -743,13 +782,16 @@
         <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E13" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="F13" t="n">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -768,46 +810,46 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>